<commit_message>
Updated excel and presentations files to reflect latest test runs
</commit_message>
<xml_diff>
--- a/Box Filter Execution TImes.xlsx
+++ b/Box Filter Execution TImes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Dropbox\School Files\3 Year\DPS915\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Dropbox\School Files\3 Year\DPS915\DPS915_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AD7D78-A22B-4EB7-ACE1-BBE318749598}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F5DA62-0A09-48F8-A854-DCA2F735255C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23220" windowHeight="8988" xr2:uid="{B52A72F4-6660-4960-B2D4-6C57F90E378C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{B52A72F4-6660-4960-B2D4-6C57F90E378C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,10 +102,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -358,28 +358,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1240</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1373</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1447</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1471</c:v>
+                  <c:v>407</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1841</c:v>
+                  <c:v>528</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2234</c:v>
+                  <c:v>754</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2752</c:v>
+                  <c:v>911</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3010</c:v>
+                  <c:v>1036</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,25 +453,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>147.63999999999999</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>203.4</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>295.83</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>401.13</c:v>
+                  <c:v>394</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>535.76</c:v>
+                  <c:v>527</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>713.55</c:v>
+                  <c:v>689</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>890.52</c:v>
+                  <c:v>904</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1121</c:v>
@@ -1674,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA21DB9-1EEA-4658-A92D-37EBC3FBC1CD}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1686,11 +1686,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
@@ -1707,112 +1707,112 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1995</v>
       </c>
       <c r="C3">
-        <v>1240</v>
+        <v>180</v>
       </c>
       <c r="D3">
-        <v>147.63999999999999</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>8028</v>
       </c>
       <c r="C4">
-        <v>1373</v>
+        <v>192</v>
       </c>
       <c r="D4">
-        <v>203.4</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>19852</v>
       </c>
       <c r="C5">
-        <v>1447</v>
+        <v>288</v>
       </c>
       <c r="D5">
-        <v>295.83</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>34278</v>
       </c>
       <c r="C6">
-        <v>1471</v>
+        <v>407</v>
       </c>
       <c r="D6">
-        <v>401.13</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>50791</v>
       </c>
       <c r="C7">
-        <v>1841</v>
+        <v>528</v>
       </c>
       <c r="D7">
-        <v>535.76</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>73605</v>
       </c>
       <c r="C8">
-        <v>2234</v>
+        <v>754</v>
       </c>
       <c r="D8">
-        <v>713.55</v>
+        <v>689</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>102737</v>
       </c>
       <c r="C9">
-        <v>2752</v>
+        <v>911</v>
       </c>
       <c r="D9">
-        <v>890.52</v>
+        <v>904</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>134687</v>
       </c>
       <c r="C10">
-        <v>3010</v>
+        <v>1036</v>
       </c>
       <c r="D10">
         <v>1121</v>

</xml_diff>